<commit_message>
BSIS-516: move defaulting of DonorStatus and isDeleted to Donor entity
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -540,8 +540,8 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
BSIS-521 Optimize donor backing form and add test data
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,302 +5,372 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Donors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>isUsageSite</t>
-  </si>
-  <si>
-    <t>isMobileSite</t>
-  </si>
-  <si>
-    <t>isVenue</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>First Location</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>externalDonorId</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>callingName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>preferredLanguage</t>
-  </si>
-  <si>
-    <t>birthDate</t>
-  </si>
-  <si>
-    <t>bloodAbo</t>
-  </si>
-  <si>
-    <t>bloodRh</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>idNumber</t>
-  </si>
-  <si>
-    <t>preferredContactType</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>homeNumber</t>
-  </si>
-  <si>
-    <t>workNumber</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>preferredAddressType</t>
-  </si>
-  <si>
-    <t>homeAddressLine1</t>
-  </si>
-  <si>
-    <t>homeAddressLine2</t>
-  </si>
-  <si>
-    <t>homeAddressCity</t>
-  </si>
-  <si>
-    <t>homeAddressProvince</t>
-  </si>
-  <si>
-    <t>homeAddressDistrict</t>
-  </si>
-  <si>
-    <t>homeAddressState</t>
-  </si>
-  <si>
-    <t>homeAddressCountry</t>
-  </si>
-  <si>
-    <t>homeAddressZipcode</t>
-  </si>
-  <si>
-    <t>workAddressLine1</t>
-  </si>
-  <si>
-    <t>workAddressLine2</t>
-  </si>
-  <si>
-    <t>workAddressCity</t>
-  </si>
-  <si>
-    <t>workAddressProvince</t>
-  </si>
-  <si>
-    <t>workAddressDistrict</t>
-  </si>
-  <si>
-    <t>workAddressCountry</t>
-  </si>
-  <si>
-    <t>workAddressState</t>
-  </si>
-  <si>
-    <t>workAddressZipcode</t>
-  </si>
-  <si>
-    <t>postalAddressLine1</t>
-  </si>
-  <si>
-    <t>postalAddressLine2</t>
-  </si>
-  <si>
-    <t>postalAddressCity</t>
-  </si>
-  <si>
-    <t>postalAddressProvince</t>
-  </si>
-  <si>
-    <t>postalAddressDistrict</t>
-  </si>
-  <si>
-    <t>postalAddressCountry</t>
-  </si>
-  <si>
-    <t>postalAddressState</t>
-  </si>
-  <si>
-    <t>postalAddressZipcode</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Imported Donor</t>
-  </si>
-  <si>
-    <t>National Id</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>0768198075</t>
-  </si>
-  <si>
-    <t>0214615177</t>
-  </si>
-  <si>
-    <t>0217010939</t>
-  </si>
-  <si>
-    <t>dave@email.com</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>1 Appartment House</t>
-  </si>
-  <si>
-    <t>123 Street</t>
-  </si>
-  <si>
-    <t>Cape Town</t>
-  </si>
-  <si>
-    <t>Western Cape</t>
-  </si>
-  <si>
-    <t>Gardens</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t>Westlake Drive</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>P.O. Box 12345</t>
-  </si>
-  <si>
-    <t>The Post Office</t>
-  </si>
-  <si>
-    <t>Vlaeberg</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Janey</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Afrikaans</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>jane@email.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isUsageSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isMobileSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isVenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDeleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalDonorId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodAbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodRh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredContactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredAddressType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0768198075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214615177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0217010939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dave@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Appartment House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box 12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Post Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlaeberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrikaans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedStartTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedEndTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorPulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haematoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -374,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,6 +467,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -424,10 +502,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.41326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.41326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.14285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.14285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,52 +618,52 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.54081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.9540816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.41326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.75"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="32.0663265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.9540816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.89285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.3775510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.6275510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.219387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.6275510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="17.6275510204082"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="22.1734693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="20.8418367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="16.7040816326531"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="20.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.41836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.02040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.14285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.47959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="31.265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.62244897959184"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.9030612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.219387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.219387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="19.1071428571429"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="17.0969387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.0408163265306"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.4387755102041"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.2397959183673"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.6428571428571"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.0204081632653"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.1071428571429"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.5663265306122"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4387755102041"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.5051020408163"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="20.3010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.3775510204082"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,6 +1077,154 @@
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>32434</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>42432</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>42432.38125</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>42432.38125</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-521 fixed donation import
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -502,10 +502,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,46 +624,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.41836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.47959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="31.265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.62244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.9030612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.219387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.219387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="19.1071428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.0408163265306"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.6428571428571"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.0204081632653"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.1071428571429"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.5663265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.3775510204082"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.28061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="30.5867346938775"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.4948979591837"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.6989795918367"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.6989795918367"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.7040816326531"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.2397959183673"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.1020408163265"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6275510204082"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.1632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.1683673469388"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.0969387755102"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.4387755102041"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.9030612244898"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,15 +1098,18 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.2551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1209,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
BSIS-521 fixed test fixtures
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -618,7 +618,7 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -1098,12 +1098,14 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.2244897959184"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8418367346939"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5765306122449"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2244897959184"/>
@@ -1206,10 +1208,10 @@
         <v>56</v>
       </c>
       <c r="L2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M2" s="0" t="n">
         <v>23</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>90</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
BSIS-521 Added current donor null checker
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>32434</v>

</xml_diff>

<commit_message>
BSIS-524: integration test for Donation import (not working)
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,354 +13,349 @@
     <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isUsageSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isMobileSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isVenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isDeleted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">externalDonorId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">callingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredLanguage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodAbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodRh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredContactType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredAddressType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imported Donor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0768198075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0214615177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0217010939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dave@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Appartment House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake Drive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.O. Box 12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Post Office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vlaeberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrikaans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jane@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">packType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedStartTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedEndTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorWeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorPulse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventComment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haematoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isUsageSite</t>
+  </si>
+  <si>
+    <t>isMobileSite</t>
+  </si>
+  <si>
+    <t>isVenue</t>
+  </si>
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>First Location</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>externalDonorId</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>callingName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>preferredLanguage</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>bloodAbo</t>
+  </si>
+  <si>
+    <t>bloodRh</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>idType</t>
+  </si>
+  <si>
+    <t>idNumber</t>
+  </si>
+  <si>
+    <t>preferredContactType</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>homeNumber</t>
+  </si>
+  <si>
+    <t>workNumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>preferredAddressType</t>
+  </si>
+  <si>
+    <t>homeAddressLine1</t>
+  </si>
+  <si>
+    <t>homeAddressLine2</t>
+  </si>
+  <si>
+    <t>homeAddressCity</t>
+  </si>
+  <si>
+    <t>homeAddressProvince</t>
+  </si>
+  <si>
+    <t>homeAddressDistrict</t>
+  </si>
+  <si>
+    <t>homeAddressState</t>
+  </si>
+  <si>
+    <t>homeAddressCountry</t>
+  </si>
+  <si>
+    <t>homeAddressZipcode</t>
+  </si>
+  <si>
+    <t>workAddressLine1</t>
+  </si>
+  <si>
+    <t>workAddressLine2</t>
+  </si>
+  <si>
+    <t>workAddressCity</t>
+  </si>
+  <si>
+    <t>workAddressProvince</t>
+  </si>
+  <si>
+    <t>workAddressDistrict</t>
+  </si>
+  <si>
+    <t>workAddressCountry</t>
+  </si>
+  <si>
+    <t>workAddressState</t>
+  </si>
+  <si>
+    <t>workAddressZipcode</t>
+  </si>
+  <si>
+    <t>postalAddressLine1</t>
+  </si>
+  <si>
+    <t>postalAddressLine2</t>
+  </si>
+  <si>
+    <t>postalAddressCity</t>
+  </si>
+  <si>
+    <t>postalAddressProvince</t>
+  </si>
+  <si>
+    <t>postalAddressDistrict</t>
+  </si>
+  <si>
+    <t>postalAddressCountry</t>
+  </si>
+  <si>
+    <t>postalAddressState</t>
+  </si>
+  <si>
+    <t>postalAddressZipcode</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Imported Donor</t>
+  </si>
+  <si>
+    <t>National Id</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>0768198075</t>
+  </si>
+  <si>
+    <t>0214615177</t>
+  </si>
+  <si>
+    <t>0217010939</t>
+  </si>
+  <si>
+    <t>dave@email.com</t>
+  </si>
+  <si>
+    <t>Home Address</t>
+  </si>
+  <si>
+    <t>1 Appartment House</t>
+  </si>
+  <si>
+    <t>123 Street</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
+  </si>
+  <si>
+    <t>Western Cape</t>
+  </si>
+  <si>
+    <t>Gardens</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t>Westlake Drive</t>
+  </si>
+  <si>
+    <t>Westlake</t>
+  </si>
+  <si>
+    <t>P.O. Box 12345</t>
+  </si>
+  <si>
+    <t>The Post Office</t>
+  </si>
+  <si>
+    <t>Vlaeberg</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Janey</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>jane@email.com</t>
+  </si>
+  <si>
+    <t>donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t>donationType</t>
+  </si>
+  <si>
+    <t>packType</t>
+  </si>
+  <si>
+    <t>donationDate</t>
+  </si>
+  <si>
+    <t>bleedStartTime</t>
+  </si>
+  <si>
+    <t>bleedEndTime</t>
+  </si>
+  <si>
+    <t>donorWeight</t>
+  </si>
+  <si>
+    <t>bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t>bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t>donorPulse</t>
+  </si>
+  <si>
+    <t>haemoglobinCount</t>
+  </si>
+  <si>
+    <t>haemoglobinLevel</t>
+  </si>
+  <si>
+    <t>adverseEventType</t>
+  </si>
+  <si>
+    <t>adverseEventComment</t>
+  </si>
+  <si>
+    <t>Voluntary</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Haematoma</t>
+  </si>
+  <si>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -368,7 +363,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
@@ -497,7 +492,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -618,8 +613,8 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -805,7 +800,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>123</v>
       </c>
@@ -1097,79 +1092,82 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8418367346939"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5459183673469"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6173469387755"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1989795918367"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.2244897959184"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BSIS-524: fixed unit test asserts
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -613,7 +613,7 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -1092,8 +1092,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1191,7 +1191,7 @@
         <v>42432</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>42432.38125</v>
+        <v>42432.375</v>
       </c>
       <c r="H2" s="7" t="n">
         <v>42432.38125</v>

</xml_diff>

<commit_message>
BSIS-541 Save donorDeferral Entity
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -249,7 +249,7 @@
     <t xml:space="preserve">dave@email.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Home</t>
+    <t xml:space="preserve">Home Address</t>
   </si>
   <si>
     <t xml:space="preserve">1 Appartment House</t>
@@ -323,7 +323,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -351,11 +351,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,7 +395,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -413,7 +408,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,10 +418,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -458,10 +449,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,16 +566,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,52 +636,52 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P48" activeCellId="0" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.41836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.47959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="31.265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.62244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.9030612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.219387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.219387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="19.1071428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.0408163265306"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.6428571428571"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.0204081632653"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.1071428571429"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.5663265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.3775510204082"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.28061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="30.5867346938775"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.4948979591837"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.6989795918367"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.6989795918367"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.7040816326531"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.2397959183673"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.5765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.1020408163265"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6275510204082"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.1632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.1683673469388"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.0969387755102"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.4387755102041"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.9030612244898"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,7 +848,7 @@
       <c r="H2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="3" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -866,7 +857,7 @@
       <c r="K2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>68</v>
       </c>
       <c r="M2" s="0" t="s">
@@ -920,10 +911,10 @@
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AE2" s="6" t="s">
         <v>83</v>
       </c>
       <c r="AF2" s="0" t="s">
@@ -994,7 +985,7 @@
       <c r="H3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="3" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
@@ -1003,7 +994,7 @@
       <c r="K3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>68</v>
       </c>
       <c r="M3" s="0" t="s">
@@ -1057,10 +1048,10 @@
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AD3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AE3" s="7" t="s">
+      <c r="AE3" s="6" t="s">
         <v>83</v>
       </c>
       <c r="AF3" s="0" t="s">

</xml_diff>

<commit_message>
BSIS-540 Validate that donor is not null
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -42,274 +42,280 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Firstds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirddsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalDonorId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReasonText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferredUntil</t>
+  </si>
+  <si>
     <t xml:space="preserve">First</t>
   </si>
   <si>
-    <t xml:space="preserve">First Location</t>
+    <t xml:space="preserve">Low weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodAbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodRh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredContactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredAddressType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0768198075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214615177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0217010939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dave@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Appartment House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box 12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Post Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlaeberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrikaans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">externalDonorId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReasonText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">createdDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferredUntil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">callingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredLanguage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodAbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodRh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredContactType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredAddressType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imported Donor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0768198075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0214615177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0217010939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dave@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Appartment House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake Drive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.O. Box 12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Post Office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vlaeberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrikaans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">jane@email.com</t>
@@ -444,7 +450,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -565,8 +571,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -600,16 +606,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>123</v>
+        <v>12366</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>42433</v>
@@ -636,8 +642,8 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P48" activeCellId="0" sqref="P48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -689,34 +695,34 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>5</v>
@@ -725,100 +731,100 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -828,133 +834,133 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AA2" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="AB2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI2" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="AE2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="AJ2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AP2" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="AQ2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -965,133 +971,133 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AA3" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="AB3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="AE3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="AJ3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP3" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AP3" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="AQ3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>

</xml_diff>

<commit_message>
BSIS-540 Fix broken build fixtures
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -42,16 +42,16 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Firstds</t>
+    <t xml:space="preserve">First</t>
   </si>
   <si>
     <t xml:space="preserve">First Location</t>
   </si>
   <si>
-    <t xml:space="preserve">Secondds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thirddsd</t>
+    <t xml:space="preserve">Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
   </si>
   <si>
     <t xml:space="preserve">externalDonorId</t>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">deferredUntil</t>
   </si>
   <si>
-    <t xml:space="preserve">First</t>
-  </si>
-  <si>
     <t xml:space="preserve">Low weight</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
   </si>
   <si>
     <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second</t>
   </si>
   <si>
     <t xml:space="preserve">jane@email.com</t>
@@ -450,15 +444,15 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.780612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,11 +571,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,16 +598,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>12366</v>
+        <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>42433</v>
@@ -648,46 +640,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.28061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.88265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="30.5867346938775"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.4948979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1683673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.6989795918367"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.7040816326531"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6275510204082"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.1632653061224"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.1683673469388"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.9030612244898"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,34 +687,34 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>5</v>
@@ -731,100 +723,100 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -834,133 +826,133 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="AG2" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="AM2" s="0" t="s">
+      <c r="AN2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AN2" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="AO2" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR2" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AR2" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -971,133 +963,133 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="S3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="T3" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="W3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="X3" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="Y3" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Z3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB3" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="AF3" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="AG3" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM3" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AN3" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AN3" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="AO3" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR3" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="AQ3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AR3" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>

</xml_diff>

<commit_message>
BSIS-524: Added checks for DonationBatch during data import. Also fixed small bug with donation batch date parsing
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
   <si>
     <t>name</t>
   </si>
@@ -49,6 +49,12 @@
     <t>Third</t>
   </si>
   <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Second venue</t>
+  </si>
+  <si>
     <t>externalDonorId</t>
   </si>
   <si>
@@ -356,6 +362,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>More notes</t>
   </si>
 </sst>
 </file>
@@ -439,12 +448,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -587,6 +600,30 @@
       <c r="E4" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +651,7 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -627,7 +664,7 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.88265306122449"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="30.5867346938775"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="30.5867346938775"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4234693877551"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.4948979591837"/>
@@ -663,139 +700,139 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -805,133 +842,133 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AD2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="AF2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AJ2" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AQ2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR2" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="AR2" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -942,133 +979,133 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="4" t="n">
+        <v>91</v>
+      </c>
+      <c r="I3" s="5" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AD3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="AF3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AJ3" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AQ3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR3" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="AR3" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
@@ -1090,10 +1127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1114,58 +1151,58 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>5</v>
@@ -1182,18 +1219,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="6" t="n">
+        <v>109</v>
+      </c>
+      <c r="F2" s="7" t="n">
         <v>42432</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="8" t="n">
         <v>42432.375</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="8" t="n">
         <v>42432.38125</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1212,22 +1249,181 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>32435</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="F3" s="7" t="n">
+        <v>42432</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>42432.3819444444</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>42432.3840277778</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="R2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>112</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>32432</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>42372</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>42372.375</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>42372.38125</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32431</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>42372</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>42372.3819444444</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>42372.3840277778</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-580 Add Outcome sheet to test fixtures
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,385 +5,400 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Donors" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Deferrals" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>isUsageSite</t>
-  </si>
-  <si>
-    <t>isMobileSite</t>
-  </si>
-  <si>
-    <t>isVenue</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>First Location</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Second venue</t>
-  </si>
-  <si>
-    <t>externalDonorId</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>callingName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>preferredLanguage</t>
-  </si>
-  <si>
-    <t>birthDate</t>
-  </si>
-  <si>
-    <t>bloodAbo</t>
-  </si>
-  <si>
-    <t>bloodRh</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>idNumber</t>
-  </si>
-  <si>
-    <t>preferredContactType</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>homeNumber</t>
-  </si>
-  <si>
-    <t>workNumber</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>preferredAddressType</t>
-  </si>
-  <si>
-    <t>homeAddressLine1</t>
-  </si>
-  <si>
-    <t>homeAddressLine2</t>
-  </si>
-  <si>
-    <t>homeAddressCity</t>
-  </si>
-  <si>
-    <t>homeAddressProvince</t>
-  </si>
-  <si>
-    <t>homeAddressDistrict</t>
-  </si>
-  <si>
-    <t>homeAddressState</t>
-  </si>
-  <si>
-    <t>homeAddressCountry</t>
-  </si>
-  <si>
-    <t>homeAddressZipcode</t>
-  </si>
-  <si>
-    <t>workAddressLine1</t>
-  </si>
-  <si>
-    <t>workAddressLine2</t>
-  </si>
-  <si>
-    <t>workAddressCity</t>
-  </si>
-  <si>
-    <t>workAddressProvince</t>
-  </si>
-  <si>
-    <t>workAddressDistrict</t>
-  </si>
-  <si>
-    <t>workAddressCountry</t>
-  </si>
-  <si>
-    <t>workAddressState</t>
-  </si>
-  <si>
-    <t>workAddressZipcode</t>
-  </si>
-  <si>
-    <t>postalAddressLine1</t>
-  </si>
-  <si>
-    <t>postalAddressLine2</t>
-  </si>
-  <si>
-    <t>postalAddressCity</t>
-  </si>
-  <si>
-    <t>postalAddressProvince</t>
-  </si>
-  <si>
-    <t>postalAddressDistrict</t>
-  </si>
-  <si>
-    <t>postalAddressCountry</t>
-  </si>
-  <si>
-    <t>postalAddressState</t>
-  </si>
-  <si>
-    <t>postalAddressZipcode</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Imported Donor</t>
-  </si>
-  <si>
-    <t>National Id</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>0768198075</t>
-  </si>
-  <si>
-    <t>0214615177</t>
-  </si>
-  <si>
-    <t>0217010939</t>
-  </si>
-  <si>
-    <t>dave@email.com</t>
-  </si>
-  <si>
-    <t>Home Address</t>
-  </si>
-  <si>
-    <t>1 Appartment House</t>
-  </si>
-  <si>
-    <t>123 Street</t>
-  </si>
-  <si>
-    <t>Cape Town</t>
-  </si>
-  <si>
-    <t>Western Cape</t>
-  </si>
-  <si>
-    <t>Gardens</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t>Westlake Drive</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>P.O. Box 12345</t>
-  </si>
-  <si>
-    <t>The Post Office</t>
-  </si>
-  <si>
-    <t>Vlaeberg</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Janey</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Afrikaans</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>jane@email.com</t>
-  </si>
-  <si>
-    <t>donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t>donationType</t>
-  </si>
-  <si>
-    <t>packType</t>
-  </si>
-  <si>
-    <t>donationDate</t>
-  </si>
-  <si>
-    <t>bleedStartTime</t>
-  </si>
-  <si>
-    <t>bleedEndTime</t>
-  </si>
-  <si>
-    <t>donorWeight</t>
-  </si>
-  <si>
-    <t>bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t>bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t>donorPulse</t>
-  </si>
-  <si>
-    <t>haemoglobinCount</t>
-  </si>
-  <si>
-    <t>haemoglobinLevel</t>
-  </si>
-  <si>
-    <t>adverseEventType</t>
-  </si>
-  <si>
-    <t>adverseEventComment</t>
-  </si>
-  <si>
-    <t>Voluntary</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Haematoma</t>
-  </si>
-  <si>
-    <t>bla</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>More notes</t>
-  </si>
-  <si>
-    <t>deferralReason</t>
-  </si>
-  <si>
-    <t>deferralReasonText</t>
-  </si>
-  <si>
-    <t>createdDate</t>
-  </si>
-  <si>
-    <t>deferredUntil</t>
-  </si>
-  <si>
-    <t>Nausea</t>
-  </si>
-  <si>
-    <t>Had nausea</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isUsageSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isMobileSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isVenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDeleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fourth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalDonorId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodAbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodRh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredContactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredAddressType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0768198075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214615177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0217010939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dave@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Appartment House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box 12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Post Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlaeberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrikaans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedStartTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedEndTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorPulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haematoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReasonText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferredUntil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nausea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had nausea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodTestName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
@@ -520,15 +535,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.780612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,51 +681,51 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.28061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.88265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="30.5867346938775"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.4948979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1683673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.6989795918367"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.7040816326531"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6275510204082"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.1632653061224"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.1683673469388"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.0969387755102"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.4387755102041"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.9030612244898"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,23 +1160,20 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5459183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.8112244897959"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,19 +1471,19 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.38775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,4 +1535,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BSIS-580 Fix outcome sheet name
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Donors" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Deferrals" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -535,15 +535,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.0204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,51 +681,51 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,20 +1160,23 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,18 +1475,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,14 +1546,15 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
BSIS-622: ensure that the BSIS-import spreadsheet fixture can be imported using initial BSIS data
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,390 +15,385 @@
     <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isUsageSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isMobileSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isVenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isDeleted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fourth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">externalDonorId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">callingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredLanguage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodAbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodRh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredContactType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredAddressType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imported Donor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0768198075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0214615177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0217010939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dave@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Appartment House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake Drive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.O. Box 12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Post Office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vlaeberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrikaans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jane@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">packType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedStartTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedEndTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorWeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorPulse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventComment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haematoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">More notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReasonText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">createdDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferredUntil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nausea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Had nausea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testedOn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodTestName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outcome</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isUsageSite</t>
+  </si>
+  <si>
+    <t>isMobileSite</t>
+  </si>
+  <si>
+    <t>isVenue</t>
+  </si>
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>First Location</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Second venue</t>
+  </si>
+  <si>
+    <t>externalDonorId</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>callingName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>preferredLanguage</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>bloodAbo</t>
+  </si>
+  <si>
+    <t>bloodRh</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>idType</t>
+  </si>
+  <si>
+    <t>idNumber</t>
+  </si>
+  <si>
+    <t>preferredContactType</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>homeNumber</t>
+  </si>
+  <si>
+    <t>workNumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>preferredAddressType</t>
+  </si>
+  <si>
+    <t>homeAddressLine1</t>
+  </si>
+  <si>
+    <t>homeAddressLine2</t>
+  </si>
+  <si>
+    <t>homeAddressCity</t>
+  </si>
+  <si>
+    <t>homeAddressProvince</t>
+  </si>
+  <si>
+    <t>homeAddressDistrict</t>
+  </si>
+  <si>
+    <t>homeAddressState</t>
+  </si>
+  <si>
+    <t>homeAddressCountry</t>
+  </si>
+  <si>
+    <t>homeAddressZipcode</t>
+  </si>
+  <si>
+    <t>workAddressLine1</t>
+  </si>
+  <si>
+    <t>workAddressLine2</t>
+  </si>
+  <si>
+    <t>workAddressCity</t>
+  </si>
+  <si>
+    <t>workAddressProvince</t>
+  </si>
+  <si>
+    <t>workAddressDistrict</t>
+  </si>
+  <si>
+    <t>workAddressCountry</t>
+  </si>
+  <si>
+    <t>workAddressState</t>
+  </si>
+  <si>
+    <t>workAddressZipcode</t>
+  </si>
+  <si>
+    <t>postalAddressLine1</t>
+  </si>
+  <si>
+    <t>postalAddressLine2</t>
+  </si>
+  <si>
+    <t>postalAddressCity</t>
+  </si>
+  <si>
+    <t>postalAddressProvince</t>
+  </si>
+  <si>
+    <t>postalAddressDistrict</t>
+  </si>
+  <si>
+    <t>postalAddressCountry</t>
+  </si>
+  <si>
+    <t>postalAddressState</t>
+  </si>
+  <si>
+    <t>postalAddressZipcode</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Imported Donor</t>
+  </si>
+  <si>
+    <t>National Id</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>0768198075</t>
+  </si>
+  <si>
+    <t>0214615177</t>
+  </si>
+  <si>
+    <t>0217010939</t>
+  </si>
+  <si>
+    <t>dave@email.com</t>
+  </si>
+  <si>
+    <t>Home Address</t>
+  </si>
+  <si>
+    <t>1 Appartment House</t>
+  </si>
+  <si>
+    <t>123 Street</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
+  </si>
+  <si>
+    <t>Western Cape</t>
+  </si>
+  <si>
+    <t>Gardens</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t>Westlake Drive</t>
+  </si>
+  <si>
+    <t>Westlake</t>
+  </si>
+  <si>
+    <t>P.O. Box 12345</t>
+  </si>
+  <si>
+    <t>The Post Office</t>
+  </si>
+  <si>
+    <t>Vlaeberg</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Janey</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>jane@email.com</t>
+  </si>
+  <si>
+    <t>donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t>donationType</t>
+  </si>
+  <si>
+    <t>packType</t>
+  </si>
+  <si>
+    <t>donationDate</t>
+  </si>
+  <si>
+    <t>bleedStartTime</t>
+  </si>
+  <si>
+    <t>bleedEndTime</t>
+  </si>
+  <si>
+    <t>donorWeight</t>
+  </si>
+  <si>
+    <t>bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t>bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t>donorPulse</t>
+  </si>
+  <si>
+    <t>haemoglobinCount</t>
+  </si>
+  <si>
+    <t>haemoglobinLevel</t>
+  </si>
+  <si>
+    <t>adverseEventType</t>
+  </si>
+  <si>
+    <t>adverseEventComment</t>
+  </si>
+  <si>
+    <t>Voluntary</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Haematoma</t>
+  </si>
+  <si>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>More notes</t>
+  </si>
+  <si>
+    <t>deferralReason</t>
+  </si>
+  <si>
+    <t>deferralReasonText</t>
+  </si>
+  <si>
+    <t>createdDate</t>
+  </si>
+  <si>
+    <t>deferredUntil</t>
+  </si>
+  <si>
+    <t>Other reasons</t>
+  </si>
+  <si>
+    <t>Had nausea</t>
+  </si>
+  <si>
+    <t>testedOn</t>
+  </si>
+  <si>
+    <t>bloodTestName</t>
+  </si>
+  <si>
+    <t>outcome</t>
   </si>
 </sst>
 </file>
@@ -406,7 +401,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
@@ -535,13 +530,16 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.37755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.48469387755102"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.0204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.56122448979592"/>
   </cols>
@@ -681,49 +679,55 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3265306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.265306122449"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8265306122449"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.93877551020408"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.8316326530612"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.9081632653061"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.6071428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.4642857142857"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1581632653061"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.765306122449"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.3316326530612"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.4642857142857"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.1530612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.4642857142857"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.6275510204082"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.7704081632653"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.6581632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.5816326530612"/>
     <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="20.7448979591837"/>
     <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.8775510204082"/>
     <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.4948979591837"/>
     <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.1224489795918"/>
   </cols>
@@ -1160,7 +1164,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1176,7 +1180,15 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,7 +1487,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1484,7 +1496,9 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,9 +1565,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.07142857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
BSIS-603 Add outcomes to import integration test
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>outcome</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>POS</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -433,6 +439,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -477,7 +488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,6 +518,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -693,6 +708,7 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8265306122449"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.93877551020408"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.8316326530612"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
@@ -1164,7 +1180,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1557,10 +1573,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1585,6 +1601,20 @@
         <v>124</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>32434</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>42445</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
BSIS-603 Check testedOn date and time separately
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -488,7 +488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,7 +521,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1180,7 +1184,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1576,13 +1580,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.07142857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
@@ -1605,8 +1610,8 @@
       <c r="A2" s="8" t="n">
         <v>32434</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>42445</v>
+      <c r="B2" s="9" t="n">
+        <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
BSIS-637 Fix donation batch grouping
The logic to group donation batches was including the time part of the
date. This change groups donation batches by the date part only so that
all donations on the same day are grouped together regardless of time.
The change to the spreadsheet adds time components to the first two
donations in order to test this case.
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,391 +15,396 @@
     <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>isUsageSite</t>
-  </si>
-  <si>
-    <t>isMobileSite</t>
-  </si>
-  <si>
-    <t>isVenue</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>First Location</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Second venue</t>
-  </si>
-  <si>
-    <t>externalDonorId</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>callingName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>preferredLanguage</t>
-  </si>
-  <si>
-    <t>birthDate</t>
-  </si>
-  <si>
-    <t>bloodAbo</t>
-  </si>
-  <si>
-    <t>bloodRh</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>idNumber</t>
-  </si>
-  <si>
-    <t>preferredContactType</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>homeNumber</t>
-  </si>
-  <si>
-    <t>workNumber</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>preferredAddressType</t>
-  </si>
-  <si>
-    <t>homeAddressLine1</t>
-  </si>
-  <si>
-    <t>homeAddressLine2</t>
-  </si>
-  <si>
-    <t>homeAddressCity</t>
-  </si>
-  <si>
-    <t>homeAddressProvince</t>
-  </si>
-  <si>
-    <t>homeAddressDistrict</t>
-  </si>
-  <si>
-    <t>homeAddressState</t>
-  </si>
-  <si>
-    <t>homeAddressCountry</t>
-  </si>
-  <si>
-    <t>homeAddressZipcode</t>
-  </si>
-  <si>
-    <t>workAddressLine1</t>
-  </si>
-  <si>
-    <t>workAddressLine2</t>
-  </si>
-  <si>
-    <t>workAddressCity</t>
-  </si>
-  <si>
-    <t>workAddressProvince</t>
-  </si>
-  <si>
-    <t>workAddressDistrict</t>
-  </si>
-  <si>
-    <t>workAddressCountry</t>
-  </si>
-  <si>
-    <t>workAddressState</t>
-  </si>
-  <si>
-    <t>workAddressZipcode</t>
-  </si>
-  <si>
-    <t>postalAddressLine1</t>
-  </si>
-  <si>
-    <t>postalAddressLine2</t>
-  </si>
-  <si>
-    <t>postalAddressCity</t>
-  </si>
-  <si>
-    <t>postalAddressProvince</t>
-  </si>
-  <si>
-    <t>postalAddressDistrict</t>
-  </si>
-  <si>
-    <t>postalAddressCountry</t>
-  </si>
-  <si>
-    <t>postalAddressState</t>
-  </si>
-  <si>
-    <t>postalAddressZipcode</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Imported Donor</t>
-  </si>
-  <si>
-    <t>National Id</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>0768198075</t>
-  </si>
-  <si>
-    <t>0214615177</t>
-  </si>
-  <si>
-    <t>0217010939</t>
-  </si>
-  <si>
-    <t>dave@email.com</t>
-  </si>
-  <si>
-    <t>Home Address</t>
-  </si>
-  <si>
-    <t>1 Appartment House</t>
-  </si>
-  <si>
-    <t>123 Street</t>
-  </si>
-  <si>
-    <t>Cape Town</t>
-  </si>
-  <si>
-    <t>Western Cape</t>
-  </si>
-  <si>
-    <t>Gardens</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t>Westlake Drive</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>P.O. Box 12345</t>
-  </si>
-  <si>
-    <t>The Post Office</t>
-  </si>
-  <si>
-    <t>Vlaeberg</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Janey</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Afrikaans</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>jane@email.com</t>
-  </si>
-  <si>
-    <t>donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t>donationType</t>
-  </si>
-  <si>
-    <t>packType</t>
-  </si>
-  <si>
-    <t>donationDate</t>
-  </si>
-  <si>
-    <t>bleedStartTime</t>
-  </si>
-  <si>
-    <t>bleedEndTime</t>
-  </si>
-  <si>
-    <t>donorWeight</t>
-  </si>
-  <si>
-    <t>bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t>bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t>donorPulse</t>
-  </si>
-  <si>
-    <t>haemoglobinCount</t>
-  </si>
-  <si>
-    <t>haemoglobinLevel</t>
-  </si>
-  <si>
-    <t>adverseEventType</t>
-  </si>
-  <si>
-    <t>adverseEventComment</t>
-  </si>
-  <si>
-    <t>Voluntary</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Haematoma</t>
-  </si>
-  <si>
-    <t>bla</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>More notes</t>
-  </si>
-  <si>
-    <t>deferralReason</t>
-  </si>
-  <si>
-    <t>deferralReasonText</t>
-  </si>
-  <si>
-    <t>createdDate</t>
-  </si>
-  <si>
-    <t>deferredUntil</t>
-  </si>
-  <si>
-    <t>Other reasons</t>
-  </si>
-  <si>
-    <t>Had nausea</t>
-  </si>
-  <si>
-    <t>testedOn</t>
-  </si>
-  <si>
-    <t>bloodTestName</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
-    <t>POS</t>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isUsageSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isMobileSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isVenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDeleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fourth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalDonorId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodAbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodRh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredContactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredAddressType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0768198075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214615177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0217010939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dave@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Appartment House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box 12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Post Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlaeberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrikaans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedStartTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedEndTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorPulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haematoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReasonText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferredUntil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had nausea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodTestName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS</t>
   </si>
 </sst>
 </file>
@@ -407,11 +412,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -439,11 +444,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -488,7 +488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,10 +525,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -554,13 +550,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.37755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.48469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,53 +699,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.6734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.6071428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.1530612244898"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.6581632653061"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.5816326530612"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,32 +1174,32 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1275510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.4387755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,7 +1278,7 @@
         <v>109</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>42432</v>
+        <v>42432.0833333333</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>42432.375</v>
@@ -1346,7 +1337,7 @@
         <v>109</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>42432</v>
+        <v>42432.5</v>
       </c>
       <c r="G3" s="7" t="n">
         <v>42432.3819444444</v>
@@ -1512,13 +1503,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,17 +1570,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.07142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1601,7 @@
       <c r="A2" s="8" t="n">
         <v>32434</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="4" t="n">
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">

</xml_diff>

<commit_message>
added unit test for minimal import of Donor, Donation and Deferral
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,396 +15,400 @@
     <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isUsageSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isMobileSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isVenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isDeleted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fourth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">externalDonorId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">callingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredLanguage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodAbo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodRh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredContactType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferredAddressType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">homeAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressLine2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressProvince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressDistrict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalAddressZipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imported Donor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0768198075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0214615177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0217010939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dave@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Appartment House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake Drive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westlake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.O. Box 12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Post Office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vlaeberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrikaans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jane@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">packType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedStartTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleedEndTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorWeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donorPulse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haemoglobinLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adverseEventComment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haematoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">More notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferralReasonText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">createdDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deferredUntil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other reasons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Had nausea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testedOn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloodTestName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isUsageSite</t>
+  </si>
+  <si>
+    <t>isMobileSite</t>
+  </si>
+  <si>
+    <t>isVenue</t>
+  </si>
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>First Location</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Second venue</t>
+  </si>
+  <si>
+    <t>externalDonorId</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>callingName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>preferredLanguage</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>bloodAbo</t>
+  </si>
+  <si>
+    <t>bloodRh</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>idType</t>
+  </si>
+  <si>
+    <t>idNumber</t>
+  </si>
+  <si>
+    <t>preferredContactType</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>homeNumber</t>
+  </si>
+  <si>
+    <t>workNumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>preferredAddressType</t>
+  </si>
+  <si>
+    <t>homeAddressLine1</t>
+  </si>
+  <si>
+    <t>homeAddressLine2</t>
+  </si>
+  <si>
+    <t>homeAddressCity</t>
+  </si>
+  <si>
+    <t>homeAddressProvince</t>
+  </si>
+  <si>
+    <t>homeAddressDistrict</t>
+  </si>
+  <si>
+    <t>homeAddressState</t>
+  </si>
+  <si>
+    <t>homeAddressCountry</t>
+  </si>
+  <si>
+    <t>homeAddressZipcode</t>
+  </si>
+  <si>
+    <t>workAddressLine1</t>
+  </si>
+  <si>
+    <t>workAddressLine2</t>
+  </si>
+  <si>
+    <t>workAddressCity</t>
+  </si>
+  <si>
+    <t>workAddressProvince</t>
+  </si>
+  <si>
+    <t>workAddressDistrict</t>
+  </si>
+  <si>
+    <t>workAddressCountry</t>
+  </si>
+  <si>
+    <t>workAddressState</t>
+  </si>
+  <si>
+    <t>workAddressZipcode</t>
+  </si>
+  <si>
+    <t>postalAddressLine1</t>
+  </si>
+  <si>
+    <t>postalAddressLine2</t>
+  </si>
+  <si>
+    <t>postalAddressCity</t>
+  </si>
+  <si>
+    <t>postalAddressProvince</t>
+  </si>
+  <si>
+    <t>postalAddressDistrict</t>
+  </si>
+  <si>
+    <t>postalAddressCountry</t>
+  </si>
+  <si>
+    <t>postalAddressState</t>
+  </si>
+  <si>
+    <t>postalAddressZipcode</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Imported Donor</t>
+  </si>
+  <si>
+    <t>National Id</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>0768198075</t>
+  </si>
+  <si>
+    <t>0214615177</t>
+  </si>
+  <si>
+    <t>0217010939</t>
+  </si>
+  <si>
+    <t>dave@email.com</t>
+  </si>
+  <si>
+    <t>Home Address</t>
+  </si>
+  <si>
+    <t>1 Appartment House</t>
+  </si>
+  <si>
+    <t>123 Street</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
+  </si>
+  <si>
+    <t>Western Cape</t>
+  </si>
+  <si>
+    <t>Gardens</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t>Westlake Drive</t>
+  </si>
+  <si>
+    <t>Westlake</t>
+  </si>
+  <si>
+    <t>P.O. Box 12345</t>
+  </si>
+  <si>
+    <t>The Post Office</t>
+  </si>
+  <si>
+    <t>Vlaeberg</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Janey</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>jane@email.com</t>
+  </si>
+  <si>
+    <t>Prof</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t>donationType</t>
+  </si>
+  <si>
+    <t>packType</t>
+  </si>
+  <si>
+    <t>donationDate</t>
+  </si>
+  <si>
+    <t>bleedStartTime</t>
+  </si>
+  <si>
+    <t>bleedEndTime</t>
+  </si>
+  <si>
+    <t>donorWeight</t>
+  </si>
+  <si>
+    <t>bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t>bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t>donorPulse</t>
+  </si>
+  <si>
+    <t>haemoglobinCount</t>
+  </si>
+  <si>
+    <t>haemoglobinLevel</t>
+  </si>
+  <si>
+    <t>adverseEventType</t>
+  </si>
+  <si>
+    <t>adverseEventComment</t>
+  </si>
+  <si>
+    <t>Voluntary</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Haematoma</t>
+  </si>
+  <si>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>More notes</t>
+  </si>
+  <si>
+    <t>deferralReason</t>
+  </si>
+  <si>
+    <t>deferralReasonText</t>
+  </si>
+  <si>
+    <t>createdDate</t>
+  </si>
+  <si>
+    <t>deferredUntil</t>
+  </si>
+  <si>
+    <t>Other reasons</t>
+  </si>
+  <si>
+    <t>Had nausea</t>
+  </si>
+  <si>
+    <t>testedOn</t>
+  </si>
+  <si>
+    <t>bloodTestName</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>POS</t>
   </si>
 </sst>
 </file>
@@ -412,7 +416,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
@@ -691,17 +695,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="1:4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
@@ -709,7 +715,8 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.1887755102041"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.5714285714286"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.280612244898"/>
@@ -741,6 +748,7 @@
     <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.2244897959184"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.5204081632653"/>
     <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,6 +1162,177 @@
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>36443</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="O4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="P4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="Q4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="R4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="S4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="T4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="U4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="V4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="W4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="X4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="Y4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="Z4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AA4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AB4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AC4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AD4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AE4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AF4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AG4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AH4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AI4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AJ4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AK4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AL4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AM4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AN4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AO4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AP4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AQ4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AR4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="AS4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1172,16 +1351,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
@@ -1207,49 +1386,49 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>21</v>
@@ -1266,16 +1445,16 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>32434</v>
+        <v>3243400</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>42432.0833333333</v>
@@ -1302,22 +1481,22 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>64</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1325,16 +1504,16 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>32435</v>
+        <v>3243500</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>42432.5</v>
@@ -1361,13 +1540,13 @@
         <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>63</v>
@@ -1376,7 +1555,7 @@
         <v>64</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,16 +1563,16 @@
         <v>123</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>32432</v>
+        <v>3243200</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>42372</v>
@@ -1420,10 +1599,10 @@
         <v>23</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>64</v>
@@ -1434,16 +1613,16 @@
         <v>456</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>32431</v>
+        <v>3243100</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>42372</v>
@@ -1470,13 +1649,83 @@
         <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="0" t="s">
         <v>63</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3243600</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>42458</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>42430.3819444445</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>42430.3888888889</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="N6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="O6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="P6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="Q6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="R6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="S6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1495,10 +1744,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1520,16 +1769,16 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,16 +1789,37 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>42372</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>42524</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>42458</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>73051</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1841,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1585,30 +1855,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="n">
-        <v>32434</v>
+        <v>3243400</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-678: fix issue in data importer where donation without ABO/Rh isn't cached and validation errors on outcomes are seen
</commit_message>
<xml_diff>
--- a/test/fixtures/BSIS-import.xlsx
+++ b/test/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
   <si>
     <t>name</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>POS</t>
+  </si>
+  <si>
+    <t>NEG</t>
   </si>
 </sst>
 </file>
@@ -1353,8 +1356,8 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1651,12 +1654,6 @@
       <c r="N5" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="Q5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1746,7 +1743,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1838,10 +1835,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1881,6 +1878,20 @@
         <v>129</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>3243100</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>42372</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>